<commit_message>
added search forms and info forms
</commit_message>
<xml_diff>
--- a/DataBased/CageDB.xlsx
+++ b/DataBased/CageDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D823C70C-DEAB-4A2B-BE25-DE8CEEA4E1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8A278F-6DBC-4253-9DE3-3F9FECE0979E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="4965" windowWidth="18855" windowHeight="16035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>CageID</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>191A</t>
+  </si>
+  <si>
+    <t>22A</t>
   </si>
 </sst>
 </file>
@@ -417,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -459,7 +462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -476,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -493,7 +496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -510,7 +513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>444</v>
       </c>
@@ -527,7 +530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -544,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>32</v>
       </c>
@@ -561,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1111</v>
       </c>
@@ -578,7 +581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -595,7 +598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -612,7 +615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>444</v>
       </c>
@@ -629,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -646,7 +649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>33</v>
       </c>
@@ -663,7 +666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>565</v>
       </c>
@@ -680,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>223</v>
       </c>
@@ -697,7 +700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -714,7 +717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5555</v>
       </c>
@@ -731,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>545</v>
       </c>
@@ -748,7 +751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -765,7 +768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -782,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -799,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -816,7 +819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -833,7 +836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -850,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -867,7 +870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>656</v>
       </c>
@@ -884,7 +887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -901,7 +904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -918,7 +921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -935,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -949,6 +952,23 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>23</v>
+      </c>
+      <c r="D32">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
databased and unit test
</commit_message>
<xml_diff>
--- a/DataBased/CageDB.xlsx
+++ b/DataBased/CageDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE638D2-CDD9-4816-868B-61C62DDF7CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50753D6D-CFA7-4C82-A474-D148CED1EA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11268" yWindow="996" windowWidth="11664" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>CageID</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>22A</t>
+  </si>
+  <si>
+    <t>453A</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -989,6 +992,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Yossi challenged me to fix few things , he doesnt know that im genius.
</commit_message>
<xml_diff>
--- a/DataBased/CageDB.xlsx
+++ b/DataBased/CageDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F27BCB5-DCC8-4BEB-80AF-7344DCE15E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFA3F9A-546C-4306-9985-EFE36BD4588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2088" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,16 +563,16 @@
         <v>444</v>
       </c>
       <c r="B6" s="1">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixxed add bird window
</commit_message>
<xml_diff>
--- a/DataBased/CageDB.xlsx
+++ b/DataBased/CageDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F27BCB5-DCC8-4BEB-80AF-7344DCE15E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF74D46-BDD2-4CE5-93CB-1E29506E16B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="11664" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>CageID</t>
   </si>
@@ -459,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
@@ -1204,6 +1204,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>250</v>
+      </c>
+      <c r="B44" s="1">
+        <v>22.55</v>
+      </c>
+      <c r="C44" s="1">
+        <v>22</v>
+      </c>
+      <c r="D44" s="1">
+        <v>22</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>